<commit_message>
fixed labels and ran code
</commit_message>
<xml_diff>
--- a/data/PCA and SD-1 plate experiment_layout.xlsx
+++ b/data/PCA and SD-1 plate experiment_layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\stillage_general_script\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB241894-D516-4146-8EA2-1F4B3CCE248C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0386317B-3255-4122-B5CC-40E811EF7329}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{32B782A3-8A08-1A41-A91D-04A3533ED90C}"/>
+    <workbookView xWindow="25170" yWindow="1170" windowWidth="18000" windowHeight="9360" xr2:uid="{32B782A3-8A08-1A41-A91D-04A3533ED90C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="68">
   <si>
     <t>96 well plate template</t>
   </si>
@@ -181,61 +181,64 @@
     <t>H20</t>
   </si>
   <si>
-    <t xml:space="preserve"> DMR+ Ferric citrate_Blk</t>
-  </si>
-  <si>
-    <t>SD-1 + mediium PIPES + Ferric Citrate_Blk</t>
-  </si>
-  <si>
-    <t>SD-1 + mediium PIPES + Ferric Citrate</t>
-  </si>
-  <si>
-    <t>SD-1 + mediium bicarb + Ferric Citrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mediium bicarb + Ferric Citrate_Blk</t>
-  </si>
-  <si>
     <t xml:space="preserve">SD-1  + DMR </t>
   </si>
   <si>
     <t>SD-1 Geo + DMR+ Ferric citrate</t>
   </si>
   <si>
-    <t>SD-1 + mediium PIPES + Ferric Citrate + lactate</t>
-  </si>
-  <si>
-    <t>SD-1 + mediium PIPES + Ferric Citrate + lactate_Blk</t>
-  </si>
-  <si>
     <t xml:space="preserve">SD-1 + AABDH medium </t>
   </si>
   <si>
     <t xml:space="preserve">SD-1 + AABDH complete </t>
   </si>
   <si>
-    <t xml:space="preserve"> AABDH medium_Blk</t>
-  </si>
-  <si>
-    <t>AABDH complete_Blk</t>
-  </si>
-  <si>
-    <t>SD-1 + DMR + Fumerate</t>
-  </si>
-  <si>
-    <t>DMR + Fumerate_Blk</t>
-  </si>
-  <si>
     <t xml:space="preserve">PCA + DMR </t>
   </si>
   <si>
-    <t>DMR_Blk</t>
-  </si>
-  <si>
-    <t>PCA + medium +Fumerate</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> medium +Fumerate_Blk</t>
+    <t xml:space="preserve">SD-1 Geo + DMR+ Ferric citrate_Blk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD-1  + DMR_Blk </t>
+  </si>
+  <si>
+    <t>SD-1 + AABDH medium_Blk</t>
+  </si>
+  <si>
+    <t>SD-1 + AABDH complete_Blk</t>
+  </si>
+  <si>
+    <t>PCA + DMR_Blk</t>
+  </si>
+  <si>
+    <t>PCA + DMR + Fumarate</t>
+  </si>
+  <si>
+    <t>PCA + medium +Fumarate</t>
+  </si>
+  <si>
+    <t>PCA + DMR + Fumarate_Blk</t>
+  </si>
+  <si>
+    <t>PCA + medium +Fumarate_Blk</t>
+  </si>
+  <si>
+    <t>SD-1 + medium bicarb + Ferric Citrate</t>
+  </si>
+  <si>
+    <t>SD-1 + medium PIPES + Ferric Citrate</t>
+  </si>
+  <si>
+    <t>SD-1 + medium PIPES + Ferric Citrate + lactate</t>
+  </si>
+  <si>
+    <t>SD-1 + medium bicarb + Ferric Citrate_Blk</t>
+  </si>
+  <si>
+    <t>SD-1 + medium PIPES + Ferric Citrate_Blk</t>
+  </si>
+  <si>
+    <t>SD-1 + medium PIPES + Ferric Citrate + lactate_Blk</t>
   </si>
 </sst>
 </file>
@@ -283,7 +286,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -372,13 +375,13 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -697,22 +700,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6812C67A-6CD4-46C1-B1B6-B8A07D368E35}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="36.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.375" customWidth="1"/>
+    <col min="11" max="11" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -760,40 +763,40 @@
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>53</v>
+      <c r="B2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>63</v>
+      <c r="J2" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="L2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -801,40 +804,40 @@
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>53</v>
+      <c r="B3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="D3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>63</v>
+      <c r="J3" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="L3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -842,40 +845,40 @@
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>53</v>
+      <c r="B4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>63</v>
+      <c r="J4" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="L4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -883,40 +886,40 @@
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>53</v>
+      <c r="B5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>63</v>
+      <c r="J5" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -924,40 +927,40 @@
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>64</v>
+      <c r="B6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>64</v>
+      <c r="J6" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="L6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -965,40 +968,40 @@
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>64</v>
+      <c r="B7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>64</v>
+      <c r="J7" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="L7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1006,40 +1009,40 @@
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>64</v>
+      <c r="B8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F8" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>64</v>
+      <c r="J8" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="L8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1047,40 +1050,40 @@
       <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>64</v>
+      <c r="B9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>64</v>
+      <c r="J9" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="L9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="M9" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1151,6 +1154,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>